<commit_message>
por eso esperaba con la carita empapada
</commit_message>
<xml_diff>
--- a/GSD/Summer2023-SedimentBaskets/SUMMER2023-SEDIMENT-BASKETS_SAND.xlsx
+++ b/GSD/Summer2023-SedimentBaskets/SUMMER2023-SEDIMENT-BASKETS_SAND.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vandalsuidaho-my.sharepoint.com/personal/huck4481_vandals_uidaho_edu/Documents/Desktop/Research/La Jara Data/Fine GSD/Sieves/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\Summer2023-SedimentBaskets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1627" documentId="8_{EED7F829-477C-4568-9838-CBD2A61330DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C23BEAA4-FF43-4379-8541-81043E5A65CF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A500C34-EE37-40EB-8007-EA8727B5A3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="360" windowWidth="23256" windowHeight="12456" xr2:uid="{209A61C2-E5C5-4D6E-B44B-8FD127605137}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{209A61C2-E5C5-4D6E-B44B-8FD127605137}"/>
   </bookViews>
   <sheets>
     <sheet name="Dry GSD (with sand)" sheetId="1" r:id="rId1"/>
@@ -947,6 +947,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -965,24 +974,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -992,13 +983,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1083,7 +1083,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1580,7 +1580,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1439155392"/>
@@ -1642,7 +1642,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015902592"/>
@@ -1684,7 +1684,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1721,7 +1721,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1797,7 +1797,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2080,7 +2080,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1439155392"/>
@@ -2142,7 +2142,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015902592"/>
@@ -2184,7 +2184,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2221,7 +2221,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2297,7 +2297,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2824,7 +2824,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1439155392"/>
@@ -2886,7 +2886,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015902592"/>
@@ -2928,7 +2928,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2965,7 +2965,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3041,7 +3041,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3530,7 +3530,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1439155392"/>
@@ -3592,7 +3592,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015902592"/>
@@ -3634,7 +3634,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3671,7 +3671,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3747,7 +3747,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4236,7 +4236,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1439155392"/>
@@ -4298,7 +4298,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015902592"/>
@@ -4340,7 +4340,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4377,7 +4377,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4587,7 +4587,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1404961039"/>
@@ -4649,7 +4649,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1226583471"/>
@@ -4697,7 +4697,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4778,7 +4778,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4953,7 +4953,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1743520911"/>
@@ -5018,7 +5018,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1736448319"/>
@@ -5066,7 +5066,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9240,9 +9240,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -9280,7 +9280,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -9386,7 +9386,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9528,7 +9528,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9538,8 +9538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF34F7D3-8706-4D54-AB6D-9CA0A6634EF9}">
   <dimension ref="A1:V129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:A98"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38:F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9567,58 +9567,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="114"/>
-      <c r="R1" s="114"/>
-      <c r="S1" s="114"/>
-      <c r="T1" s="115"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="112"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="104" t="s">
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="107" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="107" t="s">
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="110" t="s">
+      <c r="L2" s="115"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="115"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="112"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="103"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -10572,36 +10572,36 @@
     </row>
     <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:22" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="113" t="s">
+      <c r="A18" s="110" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="114"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="114"/>
-      <c r="J18" s="115"/>
-      <c r="U18" s="118"/>
-      <c r="V18" s="118"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="111"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="111"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="111"/>
+      <c r="I18" s="111"/>
+      <c r="J18" s="112"/>
+      <c r="U18" s="113"/>
+      <c r="V18" s="113"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="107" t="s">
+      <c r="A19" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="108"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="110" t="s">
+      <c r="B19" s="115"/>
+      <c r="C19" s="115"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="116"/>
+      <c r="F19" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="G19" s="111"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="111"/>
-      <c r="J19" s="112"/>
+      <c r="G19" s="102"/>
+      <c r="H19" s="102"/>
+      <c r="I19" s="102"/>
+      <c r="J19" s="103"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
@@ -10917,10 +10917,10 @@
         <f t="shared" si="16"/>
         <v>16.913600712827787</v>
       </c>
-      <c r="K27" s="118"/>
-      <c r="L27" s="118"/>
-      <c r="M27" s="118"/>
-      <c r="N27" s="118"/>
+      <c r="K27" s="113"/>
+      <c r="L27" s="113"/>
+      <c r="M27" s="113"/>
+      <c r="N27" s="113"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
@@ -11152,38 +11152,38 @@
       <c r="N34" s="1"/>
     </row>
     <row r="35" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="113" t="s">
+      <c r="A35" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="114"/>
-      <c r="C35" s="114"/>
-      <c r="D35" s="114"/>
-      <c r="E35" s="114"/>
-      <c r="F35" s="114"/>
-      <c r="G35" s="114"/>
-      <c r="H35" s="114"/>
-      <c r="I35" s="114"/>
-      <c r="J35" s="115"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="111"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="111"/>
+      <c r="G35" s="111"/>
+      <c r="H35" s="111"/>
+      <c r="I35" s="111"/>
+      <c r="J35" s="112"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="101" t="s">
+      <c r="A36" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="102"/>
-      <c r="C36" s="102"/>
-      <c r="D36" s="102"/>
-      <c r="E36" s="103"/>
-      <c r="F36" s="104" t="s">
+      <c r="B36" s="105"/>
+      <c r="C36" s="105"/>
+      <c r="D36" s="105"/>
+      <c r="E36" s="106"/>
+      <c r="F36" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="G36" s="105"/>
-      <c r="H36" s="105"/>
-      <c r="I36" s="105"/>
-      <c r="J36" s="106"/>
+      <c r="G36" s="108"/>
+      <c r="H36" s="108"/>
+      <c r="I36" s="108"/>
+      <c r="J36" s="109"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -11722,58 +11722,58 @@
       <c r="N51" s="1"/>
     </row>
     <row r="52" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="113" t="s">
+      <c r="A52" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="B52" s="114"/>
-      <c r="C52" s="114"/>
-      <c r="D52" s="114"/>
-      <c r="E52" s="114"/>
-      <c r="F52" s="114"/>
-      <c r="G52" s="114"/>
-      <c r="H52" s="114"/>
-      <c r="I52" s="114"/>
-      <c r="J52" s="114"/>
-      <c r="K52" s="114"/>
-      <c r="L52" s="114"/>
-      <c r="M52" s="114"/>
-      <c r="N52" s="114"/>
-      <c r="O52" s="114"/>
-      <c r="P52" s="114"/>
-      <c r="Q52" s="114"/>
-      <c r="R52" s="114"/>
-      <c r="S52" s="114"/>
-      <c r="T52" s="115"/>
+      <c r="B52" s="111"/>
+      <c r="C52" s="111"/>
+      <c r="D52" s="111"/>
+      <c r="E52" s="111"/>
+      <c r="F52" s="111"/>
+      <c r="G52" s="111"/>
+      <c r="H52" s="111"/>
+      <c r="I52" s="111"/>
+      <c r="J52" s="111"/>
+      <c r="K52" s="111"/>
+      <c r="L52" s="111"/>
+      <c r="M52" s="111"/>
+      <c r="N52" s="111"/>
+      <c r="O52" s="111"/>
+      <c r="P52" s="111"/>
+      <c r="Q52" s="111"/>
+      <c r="R52" s="111"/>
+      <c r="S52" s="111"/>
+      <c r="T52" s="112"/>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="101" t="s">
+      <c r="A53" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="102"/>
-      <c r="C53" s="102"/>
-      <c r="D53" s="102"/>
-      <c r="E53" s="103"/>
-      <c r="F53" s="104" t="s">
+      <c r="B53" s="105"/>
+      <c r="C53" s="105"/>
+      <c r="D53" s="105"/>
+      <c r="E53" s="106"/>
+      <c r="F53" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="105"/>
-      <c r="H53" s="105"/>
-      <c r="I53" s="105"/>
-      <c r="J53" s="116"/>
-      <c r="K53" s="107" t="s">
+      <c r="G53" s="108"/>
+      <c r="H53" s="108"/>
+      <c r="I53" s="108"/>
+      <c r="J53" s="117"/>
+      <c r="K53" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="L53" s="108"/>
-      <c r="M53" s="108"/>
-      <c r="N53" s="108"/>
-      <c r="O53" s="109"/>
-      <c r="P53" s="110" t="s">
+      <c r="L53" s="115"/>
+      <c r="M53" s="115"/>
+      <c r="N53" s="115"/>
+      <c r="O53" s="118"/>
+      <c r="P53" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="Q53" s="111"/>
-      <c r="R53" s="111"/>
-      <c r="S53" s="111"/>
-      <c r="T53" s="112"/>
+      <c r="Q53" s="102"/>
+      <c r="R53" s="102"/>
+      <c r="S53" s="102"/>
+      <c r="T53" s="103"/>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
@@ -12717,58 +12717,58 @@
     </row>
     <row r="68" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="113" t="s">
+      <c r="A69" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="B69" s="114"/>
-      <c r="C69" s="114"/>
-      <c r="D69" s="114"/>
-      <c r="E69" s="114"/>
-      <c r="F69" s="114"/>
-      <c r="G69" s="114"/>
-      <c r="H69" s="114"/>
-      <c r="I69" s="114"/>
-      <c r="J69" s="114"/>
-      <c r="K69" s="114"/>
-      <c r="L69" s="114"/>
-      <c r="M69" s="114"/>
-      <c r="N69" s="114"/>
-      <c r="O69" s="114"/>
-      <c r="P69" s="114"/>
-      <c r="Q69" s="114"/>
-      <c r="R69" s="114"/>
-      <c r="S69" s="114"/>
-      <c r="T69" s="115"/>
+      <c r="B69" s="111"/>
+      <c r="C69" s="111"/>
+      <c r="D69" s="111"/>
+      <c r="E69" s="111"/>
+      <c r="F69" s="111"/>
+      <c r="G69" s="111"/>
+      <c r="H69" s="111"/>
+      <c r="I69" s="111"/>
+      <c r="J69" s="111"/>
+      <c r="K69" s="111"/>
+      <c r="L69" s="111"/>
+      <c r="M69" s="111"/>
+      <c r="N69" s="111"/>
+      <c r="O69" s="111"/>
+      <c r="P69" s="111"/>
+      <c r="Q69" s="111"/>
+      <c r="R69" s="111"/>
+      <c r="S69" s="111"/>
+      <c r="T69" s="112"/>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" s="101" t="s">
+      <c r="A70" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="102"/>
-      <c r="C70" s="102"/>
-      <c r="D70" s="102"/>
-      <c r="E70" s="103"/>
-      <c r="F70" s="104" t="s">
+      <c r="B70" s="105"/>
+      <c r="C70" s="105"/>
+      <c r="D70" s="105"/>
+      <c r="E70" s="106"/>
+      <c r="F70" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="G70" s="105"/>
-      <c r="H70" s="105"/>
-      <c r="I70" s="105"/>
-      <c r="J70" s="116"/>
-      <c r="K70" s="107" t="s">
+      <c r="G70" s="108"/>
+      <c r="H70" s="108"/>
+      <c r="I70" s="108"/>
+      <c r="J70" s="117"/>
+      <c r="K70" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="L70" s="108"/>
-      <c r="M70" s="108"/>
-      <c r="N70" s="108"/>
-      <c r="O70" s="109"/>
-      <c r="P70" s="110" t="s">
+      <c r="L70" s="115"/>
+      <c r="M70" s="115"/>
+      <c r="N70" s="115"/>
+      <c r="O70" s="118"/>
+      <c r="P70" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="Q70" s="111"/>
-      <c r="R70" s="111"/>
-      <c r="S70" s="111"/>
-      <c r="T70" s="112"/>
+      <c r="Q70" s="102"/>
+      <c r="R70" s="102"/>
+      <c r="S70" s="102"/>
+      <c r="T70" s="103"/>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
@@ -13713,46 +13713,46 @@
     </row>
     <row r="85" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="113" t="s">
+      <c r="A86" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="B86" s="114"/>
-      <c r="C86" s="114"/>
-      <c r="D86" s="114"/>
-      <c r="E86" s="114"/>
-      <c r="F86" s="114"/>
-      <c r="G86" s="114"/>
-      <c r="H86" s="114"/>
-      <c r="I86" s="114"/>
-      <c r="J86" s="114"/>
-      <c r="K86" s="114"/>
-      <c r="L86" s="114"/>
-      <c r="M86" s="114"/>
-      <c r="N86" s="114"/>
-      <c r="O86" s="115"/>
+      <c r="B86" s="111"/>
+      <c r="C86" s="111"/>
+      <c r="D86" s="111"/>
+      <c r="E86" s="111"/>
+      <c r="F86" s="111"/>
+      <c r="G86" s="111"/>
+      <c r="H86" s="111"/>
+      <c r="I86" s="111"/>
+      <c r="J86" s="111"/>
+      <c r="K86" s="111"/>
+      <c r="L86" s="111"/>
+      <c r="M86" s="111"/>
+      <c r="N86" s="111"/>
+      <c r="O86" s="112"/>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A87" s="101" t="s">
+      <c r="A87" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="B87" s="102"/>
-      <c r="C87" s="102"/>
-      <c r="D87" s="102"/>
-      <c r="E87" s="103"/>
-      <c r="F87" s="107" t="s">
+      <c r="B87" s="105"/>
+      <c r="C87" s="105"/>
+      <c r="D87" s="105"/>
+      <c r="E87" s="106"/>
+      <c r="F87" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="G87" s="108"/>
-      <c r="H87" s="108"/>
-      <c r="I87" s="108"/>
-      <c r="J87" s="109"/>
-      <c r="K87" s="110" t="s">
+      <c r="G87" s="115"/>
+      <c r="H87" s="115"/>
+      <c r="I87" s="115"/>
+      <c r="J87" s="118"/>
+      <c r="K87" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="L87" s="111"/>
-      <c r="M87" s="111"/>
-      <c r="N87" s="111"/>
-      <c r="O87" s="112"/>
+      <c r="L87" s="102"/>
+      <c r="M87" s="102"/>
+      <c r="N87" s="102"/>
+      <c r="O87" s="103"/>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
@@ -14479,58 +14479,58 @@
       <c r="H102" s="1"/>
     </row>
     <row r="103" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="113" t="s">
+      <c r="A103" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="B103" s="114"/>
-      <c r="C103" s="114"/>
-      <c r="D103" s="114"/>
-      <c r="E103" s="114"/>
-      <c r="F103" s="114"/>
-      <c r="G103" s="114"/>
-      <c r="H103" s="114"/>
-      <c r="I103" s="114"/>
-      <c r="J103" s="114"/>
-      <c r="K103" s="114"/>
-      <c r="L103" s="114"/>
-      <c r="M103" s="114"/>
-      <c r="N103" s="114"/>
-      <c r="O103" s="114"/>
-      <c r="P103" s="114"/>
-      <c r="Q103" s="114"/>
-      <c r="R103" s="114"/>
-      <c r="S103" s="114"/>
-      <c r="T103" s="115"/>
+      <c r="B103" s="111"/>
+      <c r="C103" s="111"/>
+      <c r="D103" s="111"/>
+      <c r="E103" s="111"/>
+      <c r="F103" s="111"/>
+      <c r="G103" s="111"/>
+      <c r="H103" s="111"/>
+      <c r="I103" s="111"/>
+      <c r="J103" s="111"/>
+      <c r="K103" s="111"/>
+      <c r="L103" s="111"/>
+      <c r="M103" s="111"/>
+      <c r="N103" s="111"/>
+      <c r="O103" s="111"/>
+      <c r="P103" s="111"/>
+      <c r="Q103" s="111"/>
+      <c r="R103" s="111"/>
+      <c r="S103" s="111"/>
+      <c r="T103" s="112"/>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A104" s="101" t="s">
+      <c r="A104" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="B104" s="102"/>
-      <c r="C104" s="102"/>
-      <c r="D104" s="102"/>
-      <c r="E104" s="103"/>
-      <c r="F104" s="104" t="s">
+      <c r="B104" s="105"/>
+      <c r="C104" s="105"/>
+      <c r="D104" s="105"/>
+      <c r="E104" s="106"/>
+      <c r="F104" s="107" t="s">
         <v>50</v>
       </c>
-      <c r="G104" s="105"/>
-      <c r="H104" s="105"/>
-      <c r="I104" s="105"/>
-      <c r="J104" s="106"/>
-      <c r="K104" s="107" t="s">
+      <c r="G104" s="108"/>
+      <c r="H104" s="108"/>
+      <c r="I104" s="108"/>
+      <c r="J104" s="109"/>
+      <c r="K104" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="L104" s="108"/>
-      <c r="M104" s="108"/>
-      <c r="N104" s="108"/>
-      <c r="O104" s="109"/>
-      <c r="P104" s="110" t="s">
+      <c r="L104" s="115"/>
+      <c r="M104" s="115"/>
+      <c r="N104" s="115"/>
+      <c r="O104" s="118"/>
+      <c r="P104" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="Q104" s="111"/>
-      <c r="R104" s="111"/>
-      <c r="S104" s="111"/>
-      <c r="T104" s="112"/>
+      <c r="Q104" s="102"/>
+      <c r="R104" s="102"/>
+      <c r="S104" s="102"/>
+      <c r="T104" s="103"/>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
@@ -15486,23 +15486,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="K87:O87"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="A103:T103"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="A18:J18"/>
-    <mergeCell ref="A52:T52"/>
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="P2:T2"/>
     <mergeCell ref="A104:E104"/>
     <mergeCell ref="F104:J104"/>
     <mergeCell ref="K104:O104"/>
@@ -15519,6 +15502,23 @@
     <mergeCell ref="A86:O86"/>
     <mergeCell ref="A87:E87"/>
     <mergeCell ref="F87:J87"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A52:T52"/>
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="K87:O87"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="A103:T103"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15547,13 +15547,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="103"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="106"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">

</xml_diff>

<commit_message>
checking out weights in outlier trap pair for summer
</commit_message>
<xml_diff>
--- a/GSD/Summer2023-SedimentBaskets/SUMMER2023-SEDIMENT-BASKETS_SAND.xlsx
+++ b/GSD/Summer2023-SedimentBaskets/SUMMER2023-SEDIMENT-BASKETS_SAND.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\Summer2023-SedimentBaskets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A500C34-EE37-40EB-8007-EA8727B5A3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E1F7F2-AD69-4302-8F27-3DBFAA5DBC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{209A61C2-E5C5-4D6E-B44B-8FD127605137}"/>
   </bookViews>
@@ -691,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -947,6 +947,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9538,8 +9541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF34F7D3-8706-4D54-AB6D-9CA0A6634EF9}">
   <dimension ref="A1:V129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38:F47"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9567,58 +9570,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="111" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="112"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="113"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="107" t="s">
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="108" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="114" t="s">
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="115" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="118"/>
-      <c r="P2" s="101" t="s">
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="119"/>
+      <c r="P2" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="102"/>
-      <c r="S2" s="102"/>
-      <c r="T2" s="103"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="104"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -10457,7 +10460,6 @@
         <v>4</v>
       </c>
       <c r="L14" s="31">
-        <f>L15-L16</f>
         <v>0.21781999999999968</v>
       </c>
       <c r="M14" s="10">
@@ -10476,7 +10478,6 @@
         <v>4</v>
       </c>
       <c r="Q14" s="31">
-        <f>Q15-Q16</f>
         <v>2.0099999999999341E-2</v>
       </c>
       <c r="R14" s="10">
@@ -10518,6 +10519,10 @@
       </c>
       <c r="L15" s="55">
         <v>16.5716</v>
+      </c>
+      <c r="M15" s="101">
+        <f>SUM(L4:L13)</f>
+        <v>16.35378</v>
       </c>
       <c r="P15" s="64" t="s">
         <v>3</v>
@@ -10554,7 +10559,7 @@
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
       <c r="K16" s="25"/>
-      <c r="L16" s="26">
+      <c r="L16" s="29">
         <f>SUM(L5:L13)</f>
         <v>16.35378</v>
       </c>
@@ -10572,36 +10577,36 @@
     </row>
     <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:22" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="110" t="s">
+      <c r="A18" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="111"/>
-      <c r="C18" s="111"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="111"/>
-      <c r="J18" s="112"/>
-      <c r="U18" s="113"/>
-      <c r="V18" s="113"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="113"/>
+      <c r="U18" s="114"/>
+      <c r="V18" s="114"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="114" t="s">
+      <c r="A19" s="115" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="115"/>
-      <c r="C19" s="115"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="101" t="s">
+      <c r="B19" s="116"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="102" t="s">
         <v>78</v>
       </c>
-      <c r="G19" s="102"/>
-      <c r="H19" s="102"/>
-      <c r="I19" s="102"/>
-      <c r="J19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="103"/>
+      <c r="J19" s="104"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
@@ -10917,10 +10922,10 @@
         <f t="shared" si="16"/>
         <v>16.913600712827787</v>
       </c>
-      <c r="K27" s="113"/>
-      <c r="L27" s="113"/>
-      <c r="M27" s="113"/>
-      <c r="N27" s="113"/>
+      <c r="K27" s="114"/>
+      <c r="L27" s="114"/>
+      <c r="M27" s="114"/>
+      <c r="N27" s="114"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
@@ -11152,38 +11157,38 @@
       <c r="N34" s="1"/>
     </row>
     <row r="35" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="110" t="s">
+      <c r="A35" s="111" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="111"/>
-      <c r="C35" s="111"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="111"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="111"/>
-      <c r="I35" s="111"/>
-      <c r="J35" s="112"/>
+      <c r="B35" s="112"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="112"/>
+      <c r="G35" s="112"/>
+      <c r="H35" s="112"/>
+      <c r="I35" s="112"/>
+      <c r="J35" s="113"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="104" t="s">
+      <c r="A36" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="105"/>
-      <c r="C36" s="105"/>
-      <c r="D36" s="105"/>
-      <c r="E36" s="106"/>
-      <c r="F36" s="107" t="s">
+      <c r="B36" s="106"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="106"/>
+      <c r="E36" s="107"/>
+      <c r="F36" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="G36" s="108"/>
-      <c r="H36" s="108"/>
-      <c r="I36" s="108"/>
-      <c r="J36" s="109"/>
+      <c r="G36" s="109"/>
+      <c r="H36" s="109"/>
+      <c r="I36" s="109"/>
+      <c r="J36" s="110"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -11722,58 +11727,58 @@
       <c r="N51" s="1"/>
     </row>
     <row r="52" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="110" t="s">
+      <c r="A52" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="B52" s="111"/>
-      <c r="C52" s="111"/>
-      <c r="D52" s="111"/>
-      <c r="E52" s="111"/>
-      <c r="F52" s="111"/>
-      <c r="G52" s="111"/>
-      <c r="H52" s="111"/>
-      <c r="I52" s="111"/>
-      <c r="J52" s="111"/>
-      <c r="K52" s="111"/>
-      <c r="L52" s="111"/>
-      <c r="M52" s="111"/>
-      <c r="N52" s="111"/>
-      <c r="O52" s="111"/>
-      <c r="P52" s="111"/>
-      <c r="Q52" s="111"/>
-      <c r="R52" s="111"/>
-      <c r="S52" s="111"/>
-      <c r="T52" s="112"/>
+      <c r="B52" s="112"/>
+      <c r="C52" s="112"/>
+      <c r="D52" s="112"/>
+      <c r="E52" s="112"/>
+      <c r="F52" s="112"/>
+      <c r="G52" s="112"/>
+      <c r="H52" s="112"/>
+      <c r="I52" s="112"/>
+      <c r="J52" s="112"/>
+      <c r="K52" s="112"/>
+      <c r="L52" s="112"/>
+      <c r="M52" s="112"/>
+      <c r="N52" s="112"/>
+      <c r="O52" s="112"/>
+      <c r="P52" s="112"/>
+      <c r="Q52" s="112"/>
+      <c r="R52" s="112"/>
+      <c r="S52" s="112"/>
+      <c r="T52" s="113"/>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="104" t="s">
+      <c r="A53" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="105"/>
-      <c r="C53" s="105"/>
-      <c r="D53" s="105"/>
-      <c r="E53" s="106"/>
-      <c r="F53" s="107" t="s">
+      <c r="B53" s="106"/>
+      <c r="C53" s="106"/>
+      <c r="D53" s="106"/>
+      <c r="E53" s="107"/>
+      <c r="F53" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="108"/>
-      <c r="H53" s="108"/>
-      <c r="I53" s="108"/>
-      <c r="J53" s="117"/>
-      <c r="K53" s="114" t="s">
+      <c r="G53" s="109"/>
+      <c r="H53" s="109"/>
+      <c r="I53" s="109"/>
+      <c r="J53" s="118"/>
+      <c r="K53" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="L53" s="115"/>
-      <c r="M53" s="115"/>
-      <c r="N53" s="115"/>
-      <c r="O53" s="118"/>
-      <c r="P53" s="101" t="s">
+      <c r="L53" s="116"/>
+      <c r="M53" s="116"/>
+      <c r="N53" s="116"/>
+      <c r="O53" s="119"/>
+      <c r="P53" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="Q53" s="102"/>
-      <c r="R53" s="102"/>
-      <c r="S53" s="102"/>
-      <c r="T53" s="103"/>
+      <c r="Q53" s="103"/>
+      <c r="R53" s="103"/>
+      <c r="S53" s="103"/>
+      <c r="T53" s="104"/>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
@@ -12717,58 +12722,58 @@
     </row>
     <row r="68" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="110" t="s">
+      <c r="A69" s="111" t="s">
         <v>22</v>
       </c>
-      <c r="B69" s="111"/>
-      <c r="C69" s="111"/>
-      <c r="D69" s="111"/>
-      <c r="E69" s="111"/>
-      <c r="F69" s="111"/>
-      <c r="G69" s="111"/>
-      <c r="H69" s="111"/>
-      <c r="I69" s="111"/>
-      <c r="J69" s="111"/>
-      <c r="K69" s="111"/>
-      <c r="L69" s="111"/>
-      <c r="M69" s="111"/>
-      <c r="N69" s="111"/>
-      <c r="O69" s="111"/>
-      <c r="P69" s="111"/>
-      <c r="Q69" s="111"/>
-      <c r="R69" s="111"/>
-      <c r="S69" s="111"/>
-      <c r="T69" s="112"/>
+      <c r="B69" s="112"/>
+      <c r="C69" s="112"/>
+      <c r="D69" s="112"/>
+      <c r="E69" s="112"/>
+      <c r="F69" s="112"/>
+      <c r="G69" s="112"/>
+      <c r="H69" s="112"/>
+      <c r="I69" s="112"/>
+      <c r="J69" s="112"/>
+      <c r="K69" s="112"/>
+      <c r="L69" s="112"/>
+      <c r="M69" s="112"/>
+      <c r="N69" s="112"/>
+      <c r="O69" s="112"/>
+      <c r="P69" s="112"/>
+      <c r="Q69" s="112"/>
+      <c r="R69" s="112"/>
+      <c r="S69" s="112"/>
+      <c r="T69" s="113"/>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" s="104" t="s">
+      <c r="A70" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="105"/>
-      <c r="C70" s="105"/>
-      <c r="D70" s="105"/>
-      <c r="E70" s="106"/>
-      <c r="F70" s="107" t="s">
+      <c r="B70" s="106"/>
+      <c r="C70" s="106"/>
+      <c r="D70" s="106"/>
+      <c r="E70" s="107"/>
+      <c r="F70" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="G70" s="108"/>
-      <c r="H70" s="108"/>
-      <c r="I70" s="108"/>
-      <c r="J70" s="117"/>
-      <c r="K70" s="114" t="s">
+      <c r="G70" s="109"/>
+      <c r="H70" s="109"/>
+      <c r="I70" s="109"/>
+      <c r="J70" s="118"/>
+      <c r="K70" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="L70" s="115"/>
-      <c r="M70" s="115"/>
-      <c r="N70" s="115"/>
-      <c r="O70" s="118"/>
-      <c r="P70" s="101" t="s">
+      <c r="L70" s="116"/>
+      <c r="M70" s="116"/>
+      <c r="N70" s="116"/>
+      <c r="O70" s="119"/>
+      <c r="P70" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="Q70" s="102"/>
-      <c r="R70" s="102"/>
-      <c r="S70" s="102"/>
-      <c r="T70" s="103"/>
+      <c r="Q70" s="103"/>
+      <c r="R70" s="103"/>
+      <c r="S70" s="103"/>
+      <c r="T70" s="104"/>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
@@ -13713,46 +13718,46 @@
     </row>
     <row r="85" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="110" t="s">
+      <c r="A86" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="B86" s="111"/>
-      <c r="C86" s="111"/>
-      <c r="D86" s="111"/>
-      <c r="E86" s="111"/>
-      <c r="F86" s="111"/>
-      <c r="G86" s="111"/>
-      <c r="H86" s="111"/>
-      <c r="I86" s="111"/>
-      <c r="J86" s="111"/>
-      <c r="K86" s="111"/>
-      <c r="L86" s="111"/>
-      <c r="M86" s="111"/>
-      <c r="N86" s="111"/>
-      <c r="O86" s="112"/>
+      <c r="B86" s="112"/>
+      <c r="C86" s="112"/>
+      <c r="D86" s="112"/>
+      <c r="E86" s="112"/>
+      <c r="F86" s="112"/>
+      <c r="G86" s="112"/>
+      <c r="H86" s="112"/>
+      <c r="I86" s="112"/>
+      <c r="J86" s="112"/>
+      <c r="K86" s="112"/>
+      <c r="L86" s="112"/>
+      <c r="M86" s="112"/>
+      <c r="N86" s="112"/>
+      <c r="O86" s="113"/>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A87" s="104" t="s">
+      <c r="A87" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="B87" s="105"/>
-      <c r="C87" s="105"/>
-      <c r="D87" s="105"/>
-      <c r="E87" s="106"/>
-      <c r="F87" s="114" t="s">
+      <c r="B87" s="106"/>
+      <c r="C87" s="106"/>
+      <c r="D87" s="106"/>
+      <c r="E87" s="107"/>
+      <c r="F87" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="G87" s="115"/>
-      <c r="H87" s="115"/>
-      <c r="I87" s="115"/>
-      <c r="J87" s="118"/>
-      <c r="K87" s="101" t="s">
+      <c r="G87" s="116"/>
+      <c r="H87" s="116"/>
+      <c r="I87" s="116"/>
+      <c r="J87" s="119"/>
+      <c r="K87" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="L87" s="102"/>
-      <c r="M87" s="102"/>
-      <c r="N87" s="102"/>
-      <c r="O87" s="103"/>
+      <c r="L87" s="103"/>
+      <c r="M87" s="103"/>
+      <c r="N87" s="103"/>
+      <c r="O87" s="104"/>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
@@ -14479,58 +14484,58 @@
       <c r="H102" s="1"/>
     </row>
     <row r="103" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="110" t="s">
+      <c r="A103" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="B103" s="111"/>
-      <c r="C103" s="111"/>
-      <c r="D103" s="111"/>
-      <c r="E103" s="111"/>
-      <c r="F103" s="111"/>
-      <c r="G103" s="111"/>
-      <c r="H103" s="111"/>
-      <c r="I103" s="111"/>
-      <c r="J103" s="111"/>
-      <c r="K103" s="111"/>
-      <c r="L103" s="111"/>
-      <c r="M103" s="111"/>
-      <c r="N103" s="111"/>
-      <c r="O103" s="111"/>
-      <c r="P103" s="111"/>
-      <c r="Q103" s="111"/>
-      <c r="R103" s="111"/>
-      <c r="S103" s="111"/>
-      <c r="T103" s="112"/>
+      <c r="B103" s="112"/>
+      <c r="C103" s="112"/>
+      <c r="D103" s="112"/>
+      <c r="E103" s="112"/>
+      <c r="F103" s="112"/>
+      <c r="G103" s="112"/>
+      <c r="H103" s="112"/>
+      <c r="I103" s="112"/>
+      <c r="J103" s="112"/>
+      <c r="K103" s="112"/>
+      <c r="L103" s="112"/>
+      <c r="M103" s="112"/>
+      <c r="N103" s="112"/>
+      <c r="O103" s="112"/>
+      <c r="P103" s="112"/>
+      <c r="Q103" s="112"/>
+      <c r="R103" s="112"/>
+      <c r="S103" s="112"/>
+      <c r="T103" s="113"/>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A104" s="104" t="s">
+      <c r="A104" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="B104" s="105"/>
-      <c r="C104" s="105"/>
-      <c r="D104" s="105"/>
-      <c r="E104" s="106"/>
-      <c r="F104" s="107" t="s">
+      <c r="B104" s="106"/>
+      <c r="C104" s="106"/>
+      <c r="D104" s="106"/>
+      <c r="E104" s="107"/>
+      <c r="F104" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="G104" s="108"/>
-      <c r="H104" s="108"/>
-      <c r="I104" s="108"/>
-      <c r="J104" s="109"/>
-      <c r="K104" s="114" t="s">
+      <c r="G104" s="109"/>
+      <c r="H104" s="109"/>
+      <c r="I104" s="109"/>
+      <c r="J104" s="110"/>
+      <c r="K104" s="115" t="s">
         <v>51</v>
       </c>
-      <c r="L104" s="115"/>
-      <c r="M104" s="115"/>
-      <c r="N104" s="115"/>
-      <c r="O104" s="118"/>
-      <c r="P104" s="101" t="s">
+      <c r="L104" s="116"/>
+      <c r="M104" s="116"/>
+      <c r="N104" s="116"/>
+      <c r="O104" s="119"/>
+      <c r="P104" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="Q104" s="102"/>
-      <c r="R104" s="102"/>
-      <c r="S104" s="102"/>
-      <c r="T104" s="103"/>
+      <c r="Q104" s="103"/>
+      <c r="R104" s="103"/>
+      <c r="S104" s="103"/>
+      <c r="T104" s="104"/>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
@@ -15547,13 +15552,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="106"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="107"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">

</xml_diff>